<commit_message>
Regenerate all other representations from src
</commit_message>
<xml_diff>
--- a/project/excel/nfdi4chem_michi.xlsx
+++ b/project/excel/nfdi4chem_michi.xlsx
@@ -10,6 +10,21 @@
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dataset" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="DatasetCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RawData" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Protocol" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Characteristic" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Sample" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MaterialEntity" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="ChemicalEntity" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ChemicalSubstance" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Device" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="DevicePart" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="PlannedProcess" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="ChemicalReaction" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="ChemicalAssay" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="ChemicalAnalysis" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="SamplePreparation" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,89 +460,647 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>provenance</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>composed_of_chemical_entity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>space_group</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>iupac_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_vendor</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_serial_number</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_model_number</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_function</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_setting</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_visual_representation</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_vendor</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_serial_number</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_model_number</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_function</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_setting</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_visual_representation</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_output</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_sample</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_device</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>produces_dataset</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_output</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_status</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>based_on_assay_output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_output</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_output</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_quantitative_value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_of_analysis</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>output_of_sampling_process</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_characteristic</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>